<commit_message>
Added waterfall chart to the output excel file
</commit_message>
<xml_diff>
--- a/UK-Sales_Predictive_Model/2016/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_Analyzed_2016.xlsx
+++ b/UK-Sales_Predictive_Model/2016/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_Analyzed_2016.xlsx
@@ -4,23 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="22980" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="22980" windowHeight="9264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lasso_Weather_Output" sheetId="1" r:id="rId1"/>
+    <sheet name="UK FY16-FY17 WATERFALL" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'UK FY16-FY17 WATERFALL'!$A:$L</definedName>
+    <definedName name="valuevx">42.314159</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="47" r:id="rId3"/>
+    <pivotCache cacheId="54" r:id="rId5"/>
+    <pivotCache cacheId="57" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="187">
   <si>
     <t>Alpha_0.1</t>
   </si>
@@ -557,15 +564,41 @@
   </si>
   <si>
     <t>Sum of USD Avg. Store Daily Sales</t>
+  </si>
+  <si>
+    <t>Sales Contribution</t>
+  </si>
+  <si>
+    <t>% to Total</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>Base Sales</t>
+  </si>
+  <si>
+    <t>Clearance</t>
+  </si>
+  <si>
+    <t>Other Promos</t>
+  </si>
+  <si>
+    <t>Avg. Store Daily Sales</t>
+  </si>
+  <si>
+    <t>$1,377
+ Total Avg. Daily Store Sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -885,7 +918,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1000,6 +1033,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1047,7 +1095,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1057,6 +1105,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1104,7 +1173,26 @@
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1112,6 +1200,850 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Series 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7164291149058993E-3"/>
+                  <c:y val="-0.41945560017849176"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1800" b="1"/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>$1,377</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t> Total Avg. Daily Store Sales</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$C$53:$C$59</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Base Sales</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Holiday/Seasonality</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Clearance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B3G3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Weather</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Other Promos</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Avg. Store Daily Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$E$53:$E$59</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-43.743130379420535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>408.134485663894</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1135.3024542292396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1180.1637239157076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1218.880669266915</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1229.5946759999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1229.5946759999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Series 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Day of the Week ($230, 18.7%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9800602592868915E-3"/>
+                  <c:y val="-0.24319500223114682"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Holiday ($727, 59.1%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.4177949709864605E-3"/>
+                  <c:y val="-3.0120481927710843E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Clearance ($45, 3.6%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.0593165699542764E-4"/>
+                  <c:y val="-2.7889335118250782E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>B3G3 ($39, 3.1%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2237266279819469E-3"/>
+                  <c:y val="-2.1195894689870584E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Weather ($4, 0.3%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2237266279819469E-3"/>
+                  <c:y val="-2.3427041499330645E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Other Promos ($7, 0.6%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$C$53:$C$59</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Base Sales</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Holiday/Seasonality</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Clearance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B3G3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Weather</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Other Promos</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Avg. Store Daily Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$F$53:$F$59</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>229.97272889397277</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>727.16796856534575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.861269686467978</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.716945351207464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7861640271552872</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>6.9278427059297014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Series 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Labor ($168, 13.7%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$C$53:$C$59</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Base Sales</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Holiday/Seasonality</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Clearance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B3G3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Weather</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Other Promos</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Avg. Store Daily Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$G$53:$G$59</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>167.97290980351747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Series 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>Operating Hours ($54, 4.4%)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$C$53:$C$59</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Base Sales</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Holiday/Seasonality</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Clearance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>B3G3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Weather</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Other Promos</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Avg. Store Daily Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'UK FY16-FY17 WATERFALL'!$H$53:$H$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>53.931977345824251</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="246312320"/>
+        <c:axId val="279209088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="246312320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2800" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="279209088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="279209088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="246312320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>922020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>195634</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>126517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>157534</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>9446</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12463834" y="8904757"/>
+          <a:ext cx="1790700" cy="797329"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1"/>
+            <a:t>$408</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1"/>
+            <a:t>(Total</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+            <a:t> Base Sales)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2786,6 +3718,110 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Lasso_Weather_Output"/>
+      <sheetName val="UK FY16-FY17 WATERFALL"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="53">
+          <cell r="C53" t="str">
+            <v>Base Sales</v>
+          </cell>
+          <cell r="E53">
+            <v>-25.535000065206702</v>
+          </cell>
+          <cell r="F53">
+            <v>643.01612913364386</v>
+          </cell>
+          <cell r="G53">
+            <v>393.12999226468941</v>
+          </cell>
+          <cell r="H53">
+            <v>182.69621436264566</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="C54" t="str">
+            <v>Holiday/Seasonality</v>
+          </cell>
+          <cell r="E54">
+            <v>1193.3073356957721</v>
+          </cell>
+          <cell r="F54">
+            <v>23.488312297743846</v>
+          </cell>
+          <cell r="K54" t="str">
+            <v>Day of the Week ($643, 46.1%)</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="C55" t="str">
+            <v>Clearance</v>
+          </cell>
+          <cell r="E55">
+            <v>1216.795647993516</v>
+          </cell>
+          <cell r="F55">
+            <v>46.332734040291633</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="C56" t="str">
+            <v>B3G3</v>
+          </cell>
+          <cell r="E56">
+            <v>1263.1283820338076</v>
+          </cell>
+          <cell r="F56">
+            <v>18.921708398382446</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="C57" t="str">
+            <v>Weather</v>
+          </cell>
+          <cell r="E57">
+            <v>1282.05009043219</v>
+          </cell>
+          <cell r="F57">
+            <v>181.00522431685161</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="C58" t="str">
+            <v>Other Promos</v>
+          </cell>
+          <cell r="E58">
+            <v>1393.5054369999998</v>
+          </cell>
+          <cell r="F58">
+            <v>69.549877749041798</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="C59" t="str">
+            <v>Avg. Store Daily Sales</v>
+          </cell>
+          <cell r="E59">
+            <v>1393.5054369999998</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="K60" t="str">
+            <v>B3G3 ($19, 1.4%)</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2848,6 +3884,70 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Srini Aripirala" refreshedDate="43161.611898842595" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="153">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Lasso_Weather_Output!$A$5:$J$158"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Alpha_0.1" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1568.7816836156701" maxValue="1823.8869484638999"/>
+    </cacheField>
+    <cacheField name="Alpha_1" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-923.32651030791396" maxValue="1697.06503812406"/>
+    </cacheField>
+    <cacheField name="Alpha_10" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-634.12083606425995" maxValue="847.27570196123099"/>
+    </cacheField>
+    <cacheField name="Features" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="11">
+        <s v="Base"/>
+        <s v="Operating Hours"/>
+        <s v="Labor"/>
+        <s v="Weather"/>
+        <s v="Holiday"/>
+        <s v="Other Promo"/>
+        <s v="ES342"/>
+        <s v="B3G3"/>
+        <s v="CLX"/>
+        <s v="Day of Week"/>
+        <s v="Seasonality"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Waterfall Category" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Base"/>
+        <s v="Weather"/>
+        <s v="Holiday/Seasonality"/>
+        <s v="Other Promo"/>
+        <s v="B3G3"/>
+        <s v="CLX"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Non-Categorical Multiplier" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1" maxValue="79.505123999999995"/>
+    </cacheField>
+    <cacheField name="Contribution to Sales ($)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1568.7816836156701" maxValue="1823.8869484638999"/>
+    </cacheField>
+    <cacheField name="% to Total Betas" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.20395667359566205" maxValue="0.23712280612932829"/>
+    </cacheField>
+    <cacheField name="USD Avg. Store Daily Sales" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-250.78403998789582" maxValue="291.5649399748022"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="153">
   <r>
@@ -4689,8 +5789,1849 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="153">
+  <r>
+    <n v="-530.65433139477204"/>
+    <n v="-501.58090526613802"/>
+    <n v="-634.12083606425995"/>
+    <s v="Intercept"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="-530.65433139477204"/>
+    <n v="-6.8990155475911835E-2"/>
+    <n v="-84.829927869593433"/>
+  </r>
+  <r>
+    <n v="39.156923397578701"/>
+    <n v="33.516301300555398"/>
+    <n v="0"/>
+    <s v="Open Hours"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8.6158950000000001"/>
+    <n v="337.37194051658133"/>
+    <n v="4.3861589838100644E-2"/>
+    <n v="53.931977345824251"/>
+  </r>
+  <r>
+    <n v="50.354856953887897"/>
+    <n v="51.123607026094398"/>
+    <n v="59.283248340415099"/>
+    <s v="Labour Hours"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="20.867023"/>
+    <n v="1050.7559582184886"/>
+    <n v="0.13660835808914765"/>
+    <n v="167.97290980351747"/>
+  </r>
+  <r>
+    <n v="-15.9199573796257"/>
+    <n v="-16.430302076751701"/>
+    <n v="-44.0914878015463"/>
+    <s v="rain"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="-15.9199573796257"/>
+    <n v="-2.0697472343313233E-3"/>
+    <n v="-2.5449501799995193"/>
+  </r>
+  <r>
+    <n v="-23.029423403832102"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="snow"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="-23.029423403832102"/>
+    <n v="-2.9940460430709528E-3"/>
+    <n v="-3.6814630742589101"/>
+  </r>
+  <r>
+    <n v="2.99516290989152"/>
+    <n v="2.52648615166955"/>
+    <n v="0"/>
+    <s v="meantempi"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="50.734611999999998"/>
+    <n v="151.95842811013722"/>
+    <n v="1.9756053914868361E-2"/>
+    <n v="24.291938712491092"/>
+  </r>
+  <r>
+    <n v="-0.118441071344876"/>
+    <n v="0.95966401256647504"/>
+    <n v="2.6680023144094398"/>
+    <s v="meandewpti"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="45.045870000000001"/>
+    <n v="-5.3352811024620097"/>
+    <n v="-6.9363774304655504E-4"/>
+    <n v="-0.85289327592270003"/>
+  </r>
+  <r>
+    <n v="-2.2989190585914701"/>
+    <n v="-4.5224977544988798"/>
+    <n v="-7.3757368006350301"/>
+    <s v="meanwindspdi"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="8.3283509999999996"/>
+    <n v="-19.146204840539326"/>
+    <n v="-2.4891903647532862E-3"/>
+    <n v="-3.0606952200511386"/>
+  </r>
+  <r>
+    <n v="-0.81558492108382996"/>
+    <n v="-7.7447315177691198E-2"/>
+    <n v="5.4675541276988904"/>
+    <s v="humidity"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="79.505123999999995"/>
+    <n v="-64.843180283300114"/>
+    <n v="-8.4302357007794478E-3"/>
+    <n v="-10.365772935103537"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="precipi"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="13.2078988211801"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ash Wednesday "/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="13.2078988211801"/>
+    <n v="1.7171535956152283E-3"/>
+    <n v="2.1114029190427415"/>
+  </r>
+  <r>
+    <n v="352.17295546779201"/>
+    <n v="30.9510318416093"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Autumn Half Term Ends"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="352.17295546779201"/>
+    <n v="4.5785863818869628E-2"/>
+    <n v="56.298054387743122"/>
+  </r>
+  <r>
+    <n v="-61.839121648791597"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Autumn Half Term Starts"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-61.839121648791597"/>
+    <n v="-8.0396792500127875E-3"/>
+    <n v="-9.885546802563395"/>
+  </r>
+  <r>
+    <n v="106.315275582911"/>
+    <n v="178.95073580401399"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Bank Holiday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="106.315275582911"/>
+    <n v="1.3822006074370289E-2"/>
+    <n v="16.995465080685367"/>
+  </r>
+  <r>
+    <n v="641.83406252085103"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Bank Holiday (Easter Monday)"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="641.83406252085103"/>
+    <n v="8.3444587452369323E-2"/>
+    <n v="102.60302047244971"/>
+  </r>
+  <r>
+    <n v="-1494.2381413311"/>
+    <n v="-756.54385998660598"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Christmas Eve"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-1494.2381413311"/>
+    <n v="-0.19426529774573648"/>
+    <n v="-238.86757583971237"/>
+  </r>
+  <r>
+    <n v="-726.18215150738604"/>
+    <n v="-103.61897204129301"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Diwali"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-726.18215150738604"/>
+    <n v="-9.4410648462334032E-2"/>
+    <n v="-116.08683070699351"/>
+  </r>
+  <r>
+    <n v="-105.409196408851"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Easter Holidays End"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-105.409196408851"/>
+    <n v="-1.3704207086604407E-2"/>
+    <n v="-16.850620072490248"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Easter Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-212.22291994819699"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Easter Sunday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-212.22291994819699"/>
+    <n v="-2.7591016178639158E-2"/>
+    <n v="-33.925766598684575"/>
+  </r>
+  <r>
+    <n v="-1.18913600269974"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Eid"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-1.18913600269974"/>
+    <n v="-1.5459909182806233E-4"/>
+    <n v="-0.19009422022622052"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_England/Wales Christmas Holidays End"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-175.147456026687"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_England/Wales Christmas Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-175.147456026687"/>
+    <n v="-2.2770850076228383E-2"/>
+    <n v="-27.998916021724614"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_England/Wales Summer Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-31.4441411817781"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Father'S Day"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-31.4441411817781"/>
+    <n v="-4.088040105572132E-3"/>
+    <n v="-5.026632349085971"/>
+  </r>
+  <r>
+    <n v="66.162893219453494"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Freshers Week Starts"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="66.162893219453494"/>
+    <n v="8.601811047030717E-3"/>
+    <n v="10.576741067386955"/>
+  </r>
+  <r>
+    <n v="5.9846045845070499"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Half Term Ends"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="5.9846045845070499"/>
+    <n v="7.780560269088643E-4"/>
+    <n v="0.95669354831685227"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Half Term Starts"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="75.711828611321394"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Halloween"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="75.711828611321394"/>
+    <n v="9.8432642837975957E-3"/>
+    <n v="12.103225357818475"/>
+  </r>
+  <r>
+    <n v="29.443083292142799"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_International Womens Day                                                "/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="29.443083292142799"/>
+    <n v="3.8278833768795009E-3"/>
+    <n v="4.7067450205599357"/>
+  </r>
+  <r>
+    <n v="416.4723677197"/>
+    <n v="8.1488813373722007"/>
+    <n v="0"/>
+    <s v="Holiday_Event_May Day Bank Holiday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="416.4723677197"/>
+    <n v="5.4145404457328621E-2"/>
+    <n v="66.57690105059794"/>
+  </r>
+  <r>
+    <n v="-101.842669473513"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Mother'S Day          "/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-101.842669473513"/>
+    <n v="-1.3240524359034342E-2"/>
+    <n v="-16.28047825931694"/>
+  </r>
+  <r>
+    <n v="-182.15699130905401"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_New Years Day"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-182.15699130905401"/>
+    <n v="-2.3682156929549121E-2"/>
+    <n v="-29.119454076770104"/>
+  </r>
+  <r>
+    <n v="-1568.7816836156701"/>
+    <n v="-923.32651030791396"/>
+    <n v="0"/>
+    <s v="Holiday_Event_New Years Eve"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-1568.7816836156701"/>
+    <n v="-0.20395667359566205"/>
+    <n v="-250.78403998789582"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Bank Holiday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Christmas Holidays Ends"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-45.3930347684447"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Christmas Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-45.3930347684447"/>
+    <n v="-5.9015301316154003E-3"/>
+    <n v="-7.2564900300878747"/>
+  </r>
+  <r>
+    <n v="-86.751516831338705"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Half Term Ends"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-86.751516831338705"/>
+    <n v="-1.1278529694149978E-2"/>
+    <n v="-13.86802006503472"/>
+  </r>
+  <r>
+    <n v="49.570832951617497"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Half Term Starts"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="49.570832951617497"/>
+    <n v="6.444683987434305E-3"/>
+    <n v="7.924349119451672"/>
+  </r>
+  <r>
+    <n v="-41.157130759045003"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Holidays End"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-41.157130759045003"/>
+    <n v="-5.3508219607776896E-3"/>
+    <n v="-6.5793421951961273"/>
+  </r>
+  <r>
+    <n v="236.78957957246499"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="236.78957957246499"/>
+    <n v="3.0784917682368133E-2"/>
+    <n v="37.852970883338116"/>
+  </r>
+  <r>
+    <n v="3.5461517568710299"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni Summer Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="3.5461517568710299"/>
+    <n v="4.61033758840097E-4"/>
+    <n v="0.56688465532605115"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ni, England &amp; Wales Bank Holiday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="33.584483265312798"/>
+    <n v="0.60012328667276005"/>
+    <n v="0"/>
+    <s v="Holiday_Event_None"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="33.584483265312798"/>
+    <n v="4.3663051161046572E-3"/>
+    <n v="5.3687855245538483"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Ramadan Starts"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="460.774715048708"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Scotland Bank Holiday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="460.774715048708"/>
+    <n v="5.9905134755096283E-2"/>
+    <n v="73.659034759928943"/>
+  </r>
+  <r>
+    <n v="403.84628701934201"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Scotland Summer Holidays End"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="403.84628701934201"/>
+    <n v="5.25038928008053E-2"/>
+    <n v="64.558507057144922"/>
+  </r>
+  <r>
+    <n v="-13.0760105850394"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Scotland Summer Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-13.0760105850394"/>
+    <n v="-1.7000068592588607E-3"/>
+    <n v="-2.0903193833081763"/>
+  </r>
+  <r>
+    <n v="-246.33860235168399"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Scottish Christmas Holidays End"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-246.33860235168399"/>
+    <n v="-3.2026382280329259E-2"/>
+    <n v="-39.379469143433596"/>
+  </r>
+  <r>
+    <n v="486.96750237378399"/>
+    <n v="292.506233247046"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Scottish Christmas Holidays Start"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="486.96750237378399"/>
+    <n v="6.3310448464973759E-2"/>
+    <n v="77.846190367704097"/>
+  </r>
+  <r>
+    <n v="621.58134462184501"/>
+    <n v="50.534799415453101"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Scottish Holidays Start Bank Holiday (Good Friday)"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="621.58134462184501"/>
+    <n v="8.0811539771424731E-2"/>
+    <n v="99.365439062306095"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Shrove Tuesday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_St Patricks Day (Ni Bhol)"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="107.49850737768701"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_Valentines Day      "/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="107.49850737768701"/>
+    <n v="1.3975837562508864E-2"/>
+    <n v="17.184615459501714"/>
+  </r>
+  <r>
+    <n v="-46.107267949722903"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Event_World Book Day    "/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-46.107267949722903"/>
+    <n v="-5.994387299280317E-3"/>
+    <n v="-7.3706667090770956"/>
+  </r>
+  <r>
+    <n v="2.3207949453169698"/>
+    <n v="98.392814219024302"/>
+    <n v="0"/>
+    <s v="Holiday_Period_All School Hols"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="2.3207949453169698"/>
+    <n v="3.0172561427000815E-4"/>
+    <n v="0.37100020891923163"/>
+  </r>
+  <r>
+    <n v="42.7936818680516"/>
+    <n v="0.84265545482514803"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Bank Holiday"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="42.7936818680516"/>
+    <n v="5.5635893100196704E-3"/>
+    <n v="6.8409597950506997"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="-258.85472235064202"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Christmas"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-23.830718046650698"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Easter"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-23.830718046650698"/>
+    <n v="-3.0982220362165635E-3"/>
+    <n v="-3.8095573207977655"/>
+  </r>
+  <r>
+    <n v="-65.671564002246299"/>
+    <n v="-9.6197874699711505"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Halloween"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-65.671564002246299"/>
+    <n v="-8.5379335337804479E-3"/>
+    <n v="-10.498197617178304"/>
+  </r>
+  <r>
+    <n v="36.861757369470503"/>
+    <n v="372.82865590909302"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Halloween - School"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="36.861757369470503"/>
+    <n v="4.7923821998226762E-3"/>
+    <n v="5.8926876382591304"/>
+  </r>
+  <r>
+    <n v="577.49076372765398"/>
+    <n v="247.80743186027101"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Ni School Hols"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="577.49076372765398"/>
+    <n v="7.5079341142388026E-2"/>
+    <n v="92.317158146268071"/>
+  </r>
+  <r>
+    <n v="-13.893123584747"/>
+    <n v="-54.872085994918002"/>
+    <n v="-47.942588699695698"/>
+    <s v="Holiday_Period_Ni/England/Wales School Hols"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-13.893123584747"/>
+    <n v="-1.8062393906000181E-3"/>
+    <n v="-2.2209423382632667"/>
+  </r>
+  <r>
+    <n v="56.616452505901997"/>
+    <n v="85.1382870961653"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Ni/Scot School Hols"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="56.616452505901997"/>
+    <n v="7.3606821423850121E-3"/>
+    <n v="9.0506555740048835"/>
+  </r>
+  <r>
+    <n v="-251.006695647133"/>
+    <n v="-207.586162871471"/>
+    <n v="-175.571020897262"/>
+    <s v="Holiday_Period_None"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-251.006695647133"/>
+    <n v="-3.2633279205833678E-2"/>
+    <n v="-40.125706371914596"/>
+  </r>
+  <r>
+    <n v="107.308875497196"/>
+    <n v="67.710089641969702"/>
+    <n v="5.78088038441728"/>
+    <s v="Holiday_Period_School Hols"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="107.308875497196"/>
+    <n v="1.3951183598253305E-2"/>
+    <n v="17.154301076310787"/>
+  </r>
+  <r>
+    <n v="-72.330060851462804"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Scotland School Hols"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-72.330060851462804"/>
+    <n v="-9.4036020220709428E-3"/>
+    <n v="-11.562618981561265"/>
+  </r>
+  <r>
+    <n v="-155.09778237491599"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Period_St Patricks"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-155.09778237491599"/>
+    <n v="-2.01642000959271E-2"/>
+    <n v="-24.79379308375065"/>
+  </r>
+  <r>
+    <n v="19.250569639925601"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Holiday_Period_Valentines"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="19.250569639925601"/>
+    <n v="2.5027587902044582E-3"/>
+    <n v="3.0773788837476026"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Promo_Cc &amp; Lic"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-0.62626875818905503"/>
+    <n v="-194.94398138005701"/>
+    <n v="-178.948673970138"/>
+    <s v="Promo_Ears 342"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="-0.62626875818905503"/>
+    <n v="-8.1420948517663992E-5"/>
+    <n v="-0.10011476481218973"/>
+  </r>
+  <r>
+    <n v="40.137476528147403"/>
+    <n v="-61.780166481971698"/>
+    <n v="0"/>
+    <s v="Promo_Ears 342 &amp; Rbj Bog50% &amp; Plush Bog50%"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="40.137476528147403"/>
+    <n v="5.2182571257062427E-3"/>
+    <n v="6.4163411797674588"/>
+  </r>
+  <r>
+    <n v="-100.213424505961"/>
+    <n v="-182.22242138072701"/>
+    <n v="0"/>
+    <s v="Promo_Ears 342 &amp; Rbj Bogo50%"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="-100.213424505961"/>
+    <n v="-1.3028706878294438E-2"/>
+    <n v="-16.020028612715421"/>
+  </r>
+  <r>
+    <n v="-5.5699271227153702"/>
+    <n v="-94.629792660839897"/>
+    <n v="0"/>
+    <s v="Promo_Ears 342 / Hair 342"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="-5.5699271227153702"/>
+    <n v="-7.2414397744689253E-4"/>
+    <n v="-0.8904035793261631"/>
+  </r>
+  <r>
+    <n v="9.0880601628582198"/>
+    <n v="6.34589761639233"/>
+    <n v="0"/>
+    <s v="Promo_Es342"/>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="9.0880601628582198"/>
+    <n v="1.1815350342322792E-3"/>
+    <n v="1.4528091875994882"/>
+  </r>
+  <r>
+    <n v="97.478475384210597"/>
+    <n v="36.741554500157001"/>
+    <n v="0"/>
+    <s v="Promo_Esb3G2"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="97.478475384210597"/>
+    <n v="1.2673137246680708E-2"/>
+    <n v="15.582822086735897"/>
+  </r>
+  <r>
+    <n v="242.19417916488899"/>
+    <n v="194.89009738938401"/>
+    <n v="344.66897583228501"/>
+    <s v="Promo_Esb3G3"/>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="242.19417916488899"/>
+    <n v="3.1487567494320759E-2"/>
+    <n v="38.716945351207464"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Promo_Hair &amp; Ears 342"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-23.896061567405599"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Promo_Hair &amp; Jwly 342"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="-23.896061567405599"/>
+    <n v="-3.1067173209801402E-3"/>
+    <n v="-3.8200030777141634"/>
+  </r>
+  <r>
+    <n v="35.465881734404697"/>
+    <n v="1.9965459232512599"/>
+    <n v="0"/>
+    <s v="Promo_Hair &amp; Jwly B3G2"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="35.465881734404697"/>
+    <n v="4.6109049718217141E-3"/>
+    <n v="5.6695442048939091"/>
+  </r>
+  <r>
+    <n v="-8.5270332033212402"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Promo_Hair 342"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="-8.5270332033212402"/>
+    <n v="-1.1085961456286544E-3"/>
+    <n v="-1.3631239184991142"/>
+  </r>
+  <r>
+    <n v="344.17036982467698"/>
+    <n v="258.14787938669298"/>
+    <n v="0"/>
+    <s v="Sales_Promo_10 For 5"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="344.17036982467698"/>
+    <n v="4.4745450888899439E-2"/>
+    <n v="55.018768188210217"/>
+  </r>
+  <r>
+    <n v="-32.256977371146597"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Sales_Promo_342"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="-32.256977371146597"/>
+    <n v="-4.1937166105270353E-3"/>
+    <n v="-5.1565716169568079"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Sales_Promo_342 / Bogof"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="86.178710927408403"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Sales_Promo_345"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="86.178710927408403"/>
+    <n v="1.1204059429739241E-2"/>
+    <n v="13.776451824394966"/>
+  </r>
+  <r>
+    <n v="1.2428601272995901"/>
+    <n v="0"/>
+    <n v="43.2707906666433"/>
+    <s v="Sales_Promo_545"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="1.2428601272995901"/>
+    <n v="1.6158374358659771E-4"/>
+    <n v="0.19868251084222968"/>
+  </r>
+  <r>
+    <n v="-10.3227633384844"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Sales_Promo_75% Off"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="-10.3227633384844"/>
+    <n v="-1.3420582958236034E-3"/>
+    <n v="-1.6501877354263357"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="30.043404700213401"/>
+    <n v="0"/>
+    <s v="Sales_Promo_B3G3"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-108.382148148618"/>
+    <n v="-51.290692253130999"/>
+    <n v="0"/>
+    <s v="Sales_Promo_€2 Dot"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="-108.382148148618"/>
+    <n v="-1.4090719342539096E-2"/>
+    <n v="-17.325873484596293"/>
+  </r>
+  <r>
+    <n v="7.5086372921077102E-2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Cluster_0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="7.5086372921077102E-2"/>
+    <n v="9.7619490419153131E-6"/>
+    <n v="1.2003240569322369E-2"/>
+  </r>
+  <r>
+    <n v="-164.51088061667701"/>
+    <n v="-159.990215072914"/>
+    <n v="-111.66553123950401"/>
+    <s v="Cluster_1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="-164.51088061667701"/>
+    <n v="-2.1387993199626473E-2"/>
+    <n v="-26.298562568584913"/>
+  </r>
+  <r>
+    <n v="-25.045884286087698"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Cluster_2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="-25.045884286087698"/>
+    <n v="-3.2562053086181795E-3"/>
+    <n v="-4.0038127114398501"/>
+  </r>
+  <r>
+    <n v="446.50048779745299"/>
+    <n v="430.30866124003001"/>
+    <n v="224.77206325590299"/>
+    <s v="Cluster_3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="446.50048779745299"/>
+    <n v="5.8049348230610212E-2"/>
+    <n v="71.377169529628333"/>
+  </r>
+  <r>
+    <n v="-46.545365085294897"/>
+    <n v="-7.1036783291907604"/>
+    <n v="0"/>
+    <s v="Day_of_Week_0"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="-46.545365085294897"/>
+    <n v="-6.0513441310793177E-3"/>
+    <n v="-7.4407005262189747"/>
+  </r>
+  <r>
+    <n v="-36.055615213887002"/>
+    <n v="-22.1507565794345"/>
+    <n v="-5.0513971513708196"/>
+    <s v="Day_of_Week_1"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="-36.055615213887002"/>
+    <n v="-4.6875759834987428E-3"/>
+    <n v="-5.7638184726555179"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Day_of_Week_2"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-7.02363533924688"/>
+    <n v="-4.3543940863918804"/>
+    <n v="0"/>
+    <s v="Day_of_Week_3"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="-7.02363533924688"/>
+    <n v="-9.1313999602552734E-4"/>
+    <n v="-1.1227920775556495"/>
+  </r>
+  <r>
+    <n v="144.81717250317899"/>
+    <n v="152.71605005105999"/>
+    <n v="28.303448794549901"/>
+    <s v="Day_of_Week_4"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="144.81717250317899"/>
+    <n v="1.8827622155304043E-2"/>
+    <n v="23.150343963901495"/>
+  </r>
+  <r>
+    <n v="864.86842302362595"/>
+    <n v="825.65500317321005"/>
+    <n v="586.38060793739203"/>
+    <s v="Day_of_Week_5"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="864.86842302362595"/>
+    <n v="0.11244119465448781"/>
+    <n v="138.25709431023785"/>
+  </r>
+  <r>
+    <n v="518.53537112897595"/>
+    <n v="470.66208413702702"/>
+    <n v="234.90405443536901"/>
+    <s v="Day_of_Week_6"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="518.53537112897595"/>
+    <n v="6.7414574342434433E-2"/>
+    <n v="82.892601696263569"/>
+  </r>
+  <r>
+    <n v="-62.064135040617998"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_1"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-62.064135040617998"/>
+    <n v="-8.0689331502786406E-3"/>
+    <n v="-9.9215172425825244"/>
+  </r>
+  <r>
+    <n v="-85.085373991214496"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_2"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-85.085373991214496"/>
+    <n v="-1.1061915135887317E-2"/>
+    <n v="-13.601671957450861"/>
+  </r>
+  <r>
+    <n v="-69.683192844542404"/>
+    <n v="-46.835634438901103"/>
+    <n v="0"/>
+    <s v="Week_Num_3"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-69.683192844542404"/>
+    <n v="-9.0594837806506033E-3"/>
+    <n v="-11.139493023996334"/>
+  </r>
+  <r>
+    <n v="-43.725740838269097"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_4"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-43.725740838269097"/>
+    <n v="-5.6847659205996864E-3"/>
+    <n v="-6.9899579102756126"/>
+  </r>
+  <r>
+    <n v="-85.092271563627094"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_5"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-85.092271563627094"/>
+    <n v="-1.1062811886493122E-2"/>
+    <n v="-13.602774597221458"/>
+  </r>
+  <r>
+    <n v="-369.93369599742101"/>
+    <n v="-220.08868119916499"/>
+    <n v="0"/>
+    <s v="Week_Num_6"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-369.93369599742101"/>
+    <n v="-4.809493052767385E-2"/>
+    <n v="-59.137270519417633"/>
+  </r>
+  <r>
+    <n v="-286.705973949525"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_7"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-286.705973949525"/>
+    <n v="-3.7274527971270843E-2"/>
+    <n v="-45.832561143887709"/>
+  </r>
+  <r>
+    <n v="-66.5851663985855"/>
+    <n v="-55.0538635899428"/>
+    <n v="0"/>
+    <s v="Week_Num_8"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-66.5851663985855"/>
+    <n v="-8.6567106126388075E-3"/>
+    <n v="-10.644245280973376"/>
+  </r>
+  <r>
+    <n v="-108.418872677133"/>
+    <n v="-114.75966773376"/>
+    <n v="0"/>
+    <s v="Week_Num_9"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-108.418872677133"/>
+    <n v="-1.4095493883670929E-2"/>
+    <n v="-17.331744234952335"/>
+  </r>
+  <r>
+    <n v="-255.77732059975199"/>
+    <n v="-203.30906020418101"/>
+    <n v="0"/>
+    <s v="Week_Num_10"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-255.77732059975199"/>
+    <n v="-3.3253506230709502E-2"/>
+    <n v="-40.888334219613228"/>
+  </r>
+  <r>
+    <n v="-198.10783240987101"/>
+    <n v="-56.250070399845697"/>
+    <n v="0"/>
+    <s v="Week_Num_11"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-198.10783240987101"/>
+    <n v="-2.5755919344009216E-2"/>
+    <n v="-31.669341300879143"/>
+  </r>
+  <r>
+    <n v="-115.813251159277"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_12"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-115.813251159277"/>
+    <n v="-1.5056834046088903E-2"/>
+    <n v="-18.513802980486453"/>
+  </r>
+  <r>
+    <n v="-427.33669154769598"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_13"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-427.33669154769598"/>
+    <n v="-5.5557870813843654E-2"/>
+    <n v="-68.313662162597936"/>
+  </r>
+  <r>
+    <n v="-110.201107939275"/>
+    <n v="24.3232514856447"/>
+    <n v="0"/>
+    <s v="Week_Num_14"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-110.201107939275"/>
+    <n v="-1.4327201570870333E-2"/>
+    <n v="-17.616650773520998"/>
+  </r>
+  <r>
+    <n v="-224.954270787713"/>
+    <n v="-39.103635367249602"/>
+    <n v="0"/>
+    <s v="Week_Num_15"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-224.954270787713"/>
+    <n v="-2.9246213963472021E-2"/>
+    <n v="-35.960988982642057"/>
+  </r>
+  <r>
+    <n v="-97.822592530284595"/>
+    <n v="-1.66430080840796"/>
+    <n v="0"/>
+    <s v="Week_Num_16"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-97.822592530284595"/>
+    <n v="-1.2717875777971262E-2"/>
+    <n v="-15.637832346622821"/>
+  </r>
+  <r>
+    <n v="4.0371605250301297"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_17"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="4.0371605250301297"/>
+    <n v="5.248696106389428E-4"/>
+    <n v="0.64537687883583694"/>
+  </r>
+  <r>
+    <n v="-144.88692528996199"/>
+    <n v="-30.583828188843601"/>
+    <n v="0"/>
+    <s v="Week_Num_18"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-144.88692528996199"/>
+    <n v="-1.8836690686964547E-2"/>
+    <n v="-23.161494582150389"/>
+  </r>
+  <r>
+    <n v="-75.312620519702193"/>
+    <n v="-37.964271561691397"/>
+    <n v="0"/>
+    <s v="Week_Num_19"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-75.312620519702193"/>
+    <n v="-9.7913634009089909E-3"/>
+    <n v="-12.039408308538949"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_20"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="108.528965760159"/>
+    <n v="15.8293305360371"/>
+    <n v="0"/>
+    <s v="Week_Num_21"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="108.528965760159"/>
+    <n v="1.4109807040966418E-2"/>
+    <n v="17.349343616959622"/>
+  </r>
+  <r>
+    <n v="114.645565204505"/>
+    <n v="33.125696602522801"/>
+    <n v="0"/>
+    <s v="Week_Num_22"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="114.645565204505"/>
+    <n v="1.4905023666335631E-2"/>
+    <n v="18.327137745780291"/>
+  </r>
+  <r>
+    <n v="106.503801015075"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_23"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="106.503801015075"/>
+    <n v="1.3846516189725367E-2"/>
+    <n v="17.025602588034115"/>
+  </r>
+  <r>
+    <n v="138.08409231710601"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_24"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="138.08409231710601"/>
+    <n v="1.7952257117487387E-2"/>
+    <n v="22.073999773845596"/>
+  </r>
+  <r>
+    <n v="125.338607721248"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_25"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="125.338607721248"/>
+    <n v="1.6295221808696261E-2"/>
+    <n v="20.036517980212011"/>
+  </r>
+  <r>
+    <n v="97.109643756085106"/>
+    <n v="9.1367318582099202"/>
+    <n v="0"/>
+    <s v="Week_Num_26"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="97.109643756085106"/>
+    <n v="1.2625185595552318E-2"/>
+    <n v="15.523860991803019"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_27"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="-5.8589710549266396"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_28"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-5.8589710549266396"/>
+    <n v="-7.6172246242827573E-4"/>
+    <n v="-0.93660988439141779"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_29"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="176.94058347199299"/>
+    <n v="84.575858106642102"/>
+    <n v="0"/>
+    <s v="Week_Num_30"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="176.94058347199299"/>
+    <n v="2.3003973851765336E-2"/>
+    <n v="28.28556377497387"/>
+  </r>
+  <r>
+    <n v="12.777463686850099"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_31"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="12.777463686850099"/>
+    <n v="1.6611928975056524E-3"/>
+    <n v="2.0425939425819637"/>
+  </r>
+  <r>
+    <n v="-112.38039318673999"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_32"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-112.38039318673999"/>
+    <n v="-1.4610529566429688E-2"/>
+    <n v="-17.965029368422531"/>
+  </r>
+  <r>
+    <n v="-107.15571141089301"/>
+    <n v="-8.8171045597632602"/>
+    <n v="0"/>
+    <s v="Week_Num_33"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-107.15571141089301"/>
+    <n v="-1.3931270797203335E-2"/>
+    <n v="-17.129816402155495"/>
+  </r>
+  <r>
+    <n v="-47.874662560413398"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_34"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-47.874662560413398"/>
+    <n v="-6.2241655593735451E-3"/>
+    <n v="-7.6532008343482723"/>
+  </r>
+  <r>
+    <n v="46.732964968846602"/>
+    <n v="31.948860884009299"/>
+    <n v="0"/>
+    <s v="Week_Num_35"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="46.732964968846602"/>
+    <n v="6.0757339162328229E-3"/>
+    <n v="7.4706900761925086"/>
+  </r>
+  <r>
+    <n v="117.025815571815"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_36"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="117.025815571815"/>
+    <n v="1.5214479056025363E-2"/>
+    <n v="18.707642445402289"/>
+  </r>
+  <r>
+    <n v="96.291245097212396"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_37"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="96.291245097212396"/>
+    <n v="1.251878591618194E-2"/>
+    <n v="15.393032512521096"/>
+  </r>
+  <r>
+    <n v="92.620352871886297"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_38"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="92.620352871886297"/>
+    <n v="1.204153469937776E-2"/>
+    <n v="14.806206957224154"/>
+  </r>
+  <r>
+    <n v="59.244742646757203"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_39"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="59.244742646757203"/>
+    <n v="7.702385082935425E-3"/>
+    <n v="9.4708116904792163"/>
+  </r>
+  <r>
+    <n v="47.297796770720304"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_40"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="47.297796770720304"/>
+    <n v="6.1491674708531781E-3"/>
+    <n v="7.5609835839934529"/>
+  </r>
+  <r>
+    <n v="-82.824902110707598"/>
+    <n v="-76.293800084447099"/>
+    <n v="0"/>
+    <s v="Week_Num_41"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-82.824902110707598"/>
+    <n v="-1.0768032098929533E-2"/>
+    <n v="-13.240314939840859"/>
+  </r>
+  <r>
+    <n v="-120.818539682088"/>
+    <n v="-121.41563753949799"/>
+    <n v="0"/>
+    <s v="Week_Num_42"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-120.818539682088"/>
+    <n v="-1.5707569587025506E-2"/>
+    <n v="-19.313943937106078"/>
+  </r>
+  <r>
+    <n v="682.81442776408403"/>
+    <n v="310.956974380796"/>
+    <n v="0"/>
+    <s v="Week_Num_43"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="682.81442776408403"/>
+    <n v="8.8772428199771075E-2"/>
+    <n v="109.15410509003077"/>
+  </r>
+  <r>
+    <n v="84.690348244186893"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="Week_Num_44"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="84.690348244186893"/>
+    <n v="1.1010557997931256E-2"/>
+    <n v="13.53852349404549"/>
+  </r>
+  <r>
+    <n v="173.67842453363599"/>
+    <n v="45.270947876657097"/>
+    <n v="0"/>
+    <s v="Week_Num_45"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="173.67842453363599"/>
+    <n v="2.257986188465325E-2"/>
+    <n v="27.764077958184959"/>
+  </r>
+  <r>
+    <n v="280.90112467876401"/>
+    <n v="156.10471959284601"/>
+    <n v="0"/>
+    <s v="Week_Num_46"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="280.90112467876401"/>
+    <n v="3.6519841860160773E-2"/>
+    <n v="44.904603119615622"/>
+  </r>
+  <r>
+    <n v="434.005642461599"/>
+    <n v="346.24870195642501"/>
+    <n v="0"/>
+    <s v="Week_Num_47"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="434.005642461599"/>
+    <n v="5.642489843086524E-2"/>
+    <n v="69.379754704432656"/>
+  </r>
+  <r>
+    <n v="609.91570505171205"/>
+    <n v="528.99612343172896"/>
+    <n v="0"/>
+    <s v="Week_Num_48"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="609.91570505171205"/>
+    <n v="7.9294894678650224E-2"/>
+    <n v="97.500580330849047"/>
+  </r>
+  <r>
+    <n v="877.40321930652499"/>
+    <n v="785.85866205275704"/>
+    <n v="45.842946954816803"/>
+    <s v="Week_Num_49"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="877.40321930652499"/>
+    <n v="0.11407083846073565"/>
+    <n v="140.26089565817659"/>
+  </r>
+  <r>
+    <n v="1196.4307438329899"/>
+    <n v="1099.8894491833"/>
+    <n v="343.17149886792799"/>
+    <s v="Week_Num_50"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1196.4307438329899"/>
+    <n v="0.15554747817895984"/>
+    <n v="191.26035103407517"/>
+  </r>
+  <r>
+    <n v="1823.8869484638999"/>
+    <n v="1697.06503812406"/>
+    <n v="847.27570196123099"/>
+    <s v="Week_Num_51"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1823.8869484638999"/>
+    <n v="0.23712280612932829"/>
+    <n v="291.5649399748022"/>
+  </r>
+  <r>
+    <n v="1472.31079220638"/>
+    <n v="1377.4620013491001"/>
+    <n v="515.13578124274295"/>
+    <s v="Week_Num_52"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1472.31079220638"/>
+    <n v="0.19141453193494426"/>
+    <n v="235.36228937623943"/>
+  </r>
+  <r>
+    <n v="-358.99073626069003"/>
+    <n v="-27.034096148149299"/>
+    <n v="0"/>
+    <s v="Week_Num_53"/>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="-358.99073626069003"/>
+    <n v="-4.6672240748398167E-2"/>
+    <n v="-57.387938741220637"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="47" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="Q9:R21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -4766,6 +7707,153 @@
   <dataFields count="1">
     <dataField name="Sum of USD Avg. Store Daily Sales" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable12" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Waterfall Category">
+  <location ref="C31:E49" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="5"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sales Contribution" fld="9" baseField="0" baseItem="0" numFmtId="165"/>
+    <dataField name="% to Total" fld="9" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -5064,8 +8152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10569,4 +13657,689 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="C6:K63"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G14" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="7" customWidth="1"/>
+    <col min="11" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" customWidth="1"/>
+    <col min="14" max="14" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="7">
+        <v>52.64742943915153</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3.6636736115739831E-2</v>
+      </c>
+      <c r="H7">
+        <v>1197.51</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="7">
+        <v>139.34001609603177</v>
+      </c>
+      <c r="E8" s="8">
+        <v>9.6965102654697224E-2</v>
+      </c>
+      <c r="H8">
+        <v>1377.1364999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="7">
+        <v>59.424530024494629</v>
+      </c>
+      <c r="E9" s="8">
+        <v>4.135284188614613E-2</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.95833333333333315</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="7">
+        <v>424.34552392149624</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.29529713316346434</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="7">
+        <v>-28.613435189173781</v>
+      </c>
+      <c r="E11" s="8">
+        <v>-1.9911758001445901E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="7">
+        <v>105.18522084463977</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7.3197176394240102E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="7">
+        <v>27.987387350834663</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1.9476098564823855E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4.3635832057967319</v>
+      </c>
+      <c r="E14" s="8">
+        <v>3.0365669916442807E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="7">
+        <v>-59.350892284140279</v>
+      </c>
+      <c r="E15" s="8">
+        <v>-4.1301598235881309E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="7">
+        <v>718.41199051712738</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.49993457989016604</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="7">
+        <v>-6.7293539262584883</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-4.6828794235945752E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1437.0120000000002</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23">
+        <v>823.59721136176711</v>
+      </c>
+      <c r="E23">
+        <v>0.57313175628440616</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24">
+        <v>596.03651057415937</v>
+      </c>
+      <c r="E24">
+        <v>0.41477490137462963</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25">
+        <v>59.424530024494629</v>
+      </c>
+      <c r="E25">
+        <v>4.135284188614613E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26">
+        <v>52.64742943915153</v>
+      </c>
+      <c r="E26">
+        <v>3.6636736115739831E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27">
+        <v>-6.7293539262584883</v>
+      </c>
+      <c r="E27">
+        <v>-4.6828794235945752E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28">
+        <v>-87.964327473314057</v>
+      </c>
+      <c r="E28">
+        <v>-6.121335623732721E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29">
+        <v>1437.0120000000002</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="7">
+        <v>38.716945351207464</v>
+      </c>
+      <c r="E32" s="10">
+        <v>3.1487567494320752E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="7">
+        <v>38.716945351207464</v>
+      </c>
+      <c r="E33" s="10">
+        <v>3.1487567494320752E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="7">
+        <v>408.134485663894</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0.33192603516436658</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="7">
+        <v>229.97272889397277</v>
+      </c>
+      <c r="E35" s="10">
+        <v>0.18703133104162264</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="7">
+        <v>167.97290980351747</v>
+      </c>
+      <c r="E36" s="10">
+        <v>0.13660835808914762</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="7">
+        <v>53.931977345824251</v>
+      </c>
+      <c r="E37" s="10">
+        <v>4.3861589838100637E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="7">
+        <v>-43.743130379420535</v>
+      </c>
+      <c r="E38" s="10">
+        <v>-3.5575243804504345E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" s="7">
+        <v>44.861269686467978</v>
+      </c>
+      <c r="E39" s="10">
+        <v>3.6484599813335537E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C40" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" s="7">
+        <v>44.861269686467978</v>
+      </c>
+      <c r="E40" s="10">
+        <v>3.6484599813335537E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C41" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" s="7">
+        <v>727.16796856534575</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0.59138835159151715</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C42" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" s="7">
+        <v>-122.61191105865018</v>
+      </c>
+      <c r="E42" s="10">
+        <v>-9.9717340560972118E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C43" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" s="7">
+        <v>849.77987962399595</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0.69110569215248929</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="7">
+        <v>6.9278427059297014</v>
+      </c>
+      <c r="E44" s="10">
+        <v>5.6342491075731535E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C45" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1.4528091875994882</v>
+      </c>
+      <c r="E45" s="10">
+        <v>1.181535034232279E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C46" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="7">
+        <v>5.4750335183302132</v>
+      </c>
+      <c r="E46" s="10">
+        <v>4.4527140733408741E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="7">
+        <v>3.7861640271552872</v>
+      </c>
+      <c r="E47" s="10">
+        <v>3.0791968288867953E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C48" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="7">
+        <v>3.7861640271552872</v>
+      </c>
+      <c r="E48" s="10">
+        <v>3.0791968288867953E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C49" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D49" s="7">
+        <v>1229.5946760000002</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C53" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="13">
+        <f>D34</f>
+        <v>408.134485663894</v>
+      </c>
+      <c r="E53" s="13">
+        <f>D38</f>
+        <v>-43.743130379420535</v>
+      </c>
+      <c r="F53" s="13">
+        <f>D35</f>
+        <v>229.97272889397277</v>
+      </c>
+      <c r="G53" s="13">
+        <f>D36</f>
+        <v>167.97290980351747</v>
+      </c>
+      <c r="H53" s="13">
+        <f>D37</f>
+        <v>53.931977345824251</v>
+      </c>
+      <c r="I53" s="14"/>
+      <c r="J53">
+        <f>D53/$E$59</f>
+        <v>0.33192603516436664</v>
+      </c>
+      <c r="K53" t="str">
+        <f>"Base ($"&amp;TEXT(E53,"###")&amp;", "&amp;TEXT(E38*100,"#.#")&amp;"%)"</f>
+        <v>Base ($-44, -3.6%)</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C54" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="13">
+        <f>D41</f>
+        <v>727.16796856534575</v>
+      </c>
+      <c r="E54" s="7">
+        <f>D53</f>
+        <v>408.134485663894</v>
+      </c>
+      <c r="F54" s="7">
+        <f>D41</f>
+        <v>727.16796856534575</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="J54">
+        <f t="shared" ref="J54:J58" si="0">D54/$E$59</f>
+        <v>0.59138835159151726</v>
+      </c>
+      <c r="K54" t="str">
+        <f>"Day of the Week ($"&amp;TEXT(F53,"###")&amp;", "&amp;TEXT(E35*100,"#.#")&amp;"%)"</f>
+        <v>Day of the Week ($230, 18.7%)</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C55" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D55" s="13">
+        <f>D39</f>
+        <v>44.861269686467978</v>
+      </c>
+      <c r="E55" s="7">
+        <f>SUM(D53:D54)</f>
+        <v>1135.3024542292396</v>
+      </c>
+      <c r="F55" s="7">
+        <f>D55</f>
+        <v>44.861269686467978</v>
+      </c>
+      <c r="G55" s="7"/>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>3.6484599813335544E-2</v>
+      </c>
+      <c r="K55" t="str">
+        <f>"Labor ($"&amp;TEXT(G53,"###")&amp;", "&amp;TEXT(E36*100,"#.#")&amp;"%)"</f>
+        <v>Labor ($168, 13.7%)</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C56" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="13">
+        <f>D32</f>
+        <v>38.716945351207464</v>
+      </c>
+      <c r="E56" s="7">
+        <f>SUM(E55:F55)</f>
+        <v>1180.1637239157076</v>
+      </c>
+      <c r="F56" s="7">
+        <f>D56</f>
+        <v>38.716945351207464</v>
+      </c>
+      <c r="G56" s="7"/>
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>3.1487567494320759E-2</v>
+      </c>
+      <c r="K56" t="str">
+        <f>"Operating Hours ($"&amp;TEXT(H53,"###")&amp;", "&amp;TEXT(E37*100,"#.#")&amp;"%)"</f>
+        <v>Operating Hours ($54, 4.4%)</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C57" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="13">
+        <f>D47</f>
+        <v>3.7861640271552872</v>
+      </c>
+      <c r="E57" s="7">
+        <f>SUM(E56:F56)</f>
+        <v>1218.880669266915</v>
+      </c>
+      <c r="F57" s="7">
+        <f>D57</f>
+        <v>3.7861640271552872</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>3.0791968288867962E-3</v>
+      </c>
+      <c r="K57" t="str">
+        <f>"Seasonality ($"&amp;TEXT(F54,"###")&amp;", "&amp;TEXT(E43*100,"#.#")&amp;"%)"</f>
+        <v>Seasonality ($727, 69.1%)</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C58" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D58" s="13">
+        <f>D44</f>
+        <v>6.9278427059297014</v>
+      </c>
+      <c r="E58" s="7">
+        <f>SUM(E57:F57,D58)</f>
+        <v>1229.5946759999999</v>
+      </c>
+      <c r="F58" s="3">
+        <f>D58</f>
+        <v>6.9278427059297014</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>5.6342491075731544E-3</v>
+      </c>
+      <c r="K58" t="str">
+        <f>"Holiday ($"&amp;TEXT(G54,"###")&amp;", "&amp;TEXT(E42*100,"#.#")&amp;"%)"</f>
+        <v>Holiday ($, -10.%)</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C59" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="E59" s="7">
+        <f>SUM(D53:D58)</f>
+        <v>1229.5946759999999</v>
+      </c>
+      <c r="K59" t="str">
+        <f>"Clearance ($"&amp;TEXT(F55,"###")&amp;", "&amp;TEXT(E39*100,"#.#")&amp;"%)"</f>
+        <v>Clearance ($45, 3.6%)</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D60" s="13"/>
+      <c r="K60" t="str">
+        <f>"B3G3 ($"&amp;TEXT(F56,"###")&amp;", "&amp;TEXT(E32*100,"#.#")&amp;"%)"</f>
+        <v>B3G3 ($39, 3.1%)</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="K61" t="str">
+        <f>"Weather ($"&amp;TEXT(F57,"###")&amp;", "&amp;TEXT(E47*100,"#.#")&amp;"%)"</f>
+        <v>Weather ($4, .3%)</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="K62" t="str">
+        <f>"Other Promos ($"&amp;TEXT(F58,"###")&amp;", "&amp;TEXT(E46*100,"#.#")&amp;"%)"</f>
+        <v>Other Promos ($7, .4%)</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K63" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;8&amp;K01+049http://www.vertex42.com/ExcelTemplates/waterfall-chart.html&amp;R&amp;"Arial,Regular"&amp;8&amp;K01+049Waterfall Chart Template by Vertex42.com</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>